<commit_message>
update data and data_preprocess_1
</commit_message>
<xml_diff>
--- a/data/insomnia_and_sleep_quality_node.xlsx
+++ b/data/insomnia_and_sleep_quality_node.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3240" yWindow="2316" windowWidth="17280" windowHeight="9420" tabRatio="600" firstSheet="3" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3435" yWindow="4350" windowWidth="21600" windowHeight="11775" tabRatio="600" firstSheet="2" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MAIN" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MENSTRUAL_INSOMNIA" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INSOMNIA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MENOPAUSE_INSOMNIA" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GAD_7" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -470,19 +471,19 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col width="20.8984375" customWidth="1" style="7" min="1" max="1"/>
-    <col width="18.8984375" customWidth="1" style="6" min="2" max="3"/>
-    <col width="14.8984375" customWidth="1" style="6" min="4" max="4"/>
+    <col width="20.875" customWidth="1" style="7" min="1" max="1"/>
+    <col width="18.875" customWidth="1" style="6" min="2" max="3"/>
+    <col width="14.875" customWidth="1" style="6" min="4" max="4"/>
     <col width="17" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
     <col width="32" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="11" customWidth="1" style="6" min="7" max="19"/>
-    <col width="11" customWidth="1" style="6" min="20" max="16384"/>
+    <col width="11" customWidth="1" style="6" min="7" max="23"/>
+    <col width="11" customWidth="1" style="6" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1647,16 +1648,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col width="23.19921875" customWidth="1" style="8" min="1" max="1"/>
-    <col width="21.19921875" customWidth="1" style="8" min="2" max="2"/>
+    <col width="23.25" customWidth="1" style="8" min="1" max="1"/>
+    <col width="21.25" customWidth="1" style="8" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="6">
@@ -3713,6 +3714,142 @@
       <c r="C121" s="6" t="inlineStr">
         <is>
           <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="6" t="inlineStr">
+        <is>
+          <t>Feeling_nervous__anxious__or_anxious</t>
+        </is>
+      </c>
+      <c r="B122" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C122" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="6" t="inlineStr">
+        <is>
+          <t>Inability_to_stop_or_control_worry</t>
+        </is>
+      </c>
+      <c r="B123" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C123" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="6" t="inlineStr">
+        <is>
+          <t>Worrying_too_much_about_all_kinds_of_things</t>
+        </is>
+      </c>
+      <c r="B124" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C124" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="6" t="inlineStr">
+        <is>
+          <t>Hard_to_relax</t>
+        </is>
+      </c>
+      <c r="B125" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C125" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="6" t="inlineStr">
+        <is>
+          <t>Unable_to_sit_still_due_to_restlessness</t>
+        </is>
+      </c>
+      <c r="B126" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C126" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="6" t="inlineStr">
+        <is>
+          <t>Become_easily_irritable_or_irritable</t>
+        </is>
+      </c>
+      <c r="B127" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C127" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="6" t="inlineStr">
+        <is>
+          <t>Fear_that_something_terrible_is_about_to_happen</t>
+        </is>
+      </c>
+      <c r="B128" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+      <c r="C128" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_</t>
+        </is>
+      </c>
+      <c r="B129" s="6" t="inlineStr">
+        <is>
+          <t>QUESTIONNAIRE</t>
+        </is>
+      </c>
+      <c r="C129" s="6" t="inlineStr">
+        <is>
+          <t>MAIN</t>
         </is>
       </c>
     </row>
@@ -3729,16 +3866,16 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col width="19.09765625" customWidth="1" style="8" min="1" max="1"/>
-    <col width="18.796875" customWidth="1" style="8" min="2" max="2"/>
-    <col width="12.19921875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.796875" customWidth="1" style="8" min="4" max="4"/>
+    <col width="19.125" customWidth="1" style="8" min="1" max="1"/>
+    <col width="18.75" customWidth="1" style="8" min="2" max="2"/>
+    <col width="12.25" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.75" customWidth="1" style="8" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4193,15 +4330,15 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
     <col width="19" customWidth="1" style="8" min="1" max="1"/>
     <col width="15.5" customWidth="1" style="8" min="2" max="2"/>
-    <col width="12.19921875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="16.69921875" customWidth="1" style="8" min="5" max="5"/>
+    <col width="12.25" customWidth="1" style="8" min="3" max="3"/>
+    <col width="16.75" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4483,16 +4620,16 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col width="20.59765625" customWidth="1" style="8" min="1" max="1"/>
-    <col width="15.796875" customWidth="1" style="8" min="2" max="2"/>
-    <col width="8.796875" customWidth="1" style="6" min="3" max="3"/>
-    <col width="22.59765625" customWidth="1" style="8" min="5" max="5"/>
+    <col width="20.625" customWidth="1" style="8" min="1" max="1"/>
+    <col width="15.75" customWidth="1" style="8" min="2" max="2"/>
+    <col width="8.75" customWidth="1" style="6" min="3" max="3"/>
+    <col width="22.625" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5161,15 +5298,15 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col width="23.296875" customWidth="1" style="8" min="1" max="1"/>
-    <col width="25.796875" customWidth="1" style="8" min="2" max="3"/>
-    <col width="34.796875" customWidth="1" style="8" min="5" max="5"/>
+    <col width="23.25" customWidth="1" style="8" min="1" max="1"/>
+    <col width="25.75" customWidth="1" style="8" min="2" max="3"/>
+    <col width="34.75" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5621,4 +5758,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <cols>
+    <col width="29.375" customWidth="1" style="8" min="1" max="1"/>
+    <col width="24.125" customWidth="1" style="8" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>ChineseName</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>EnglishName</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Classification</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Abbreviation</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>CorrespondingReason</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>感觉紧张，焦虑或急切</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Feeling_nervous__anxious__or_anxious</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>不能够停止或控制担忧</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Inability_to_stop_or_control_worry</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>对各种各样的事情担忧过多</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Worrying_too_much_about_all_kinds_of_things</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>很难放松下来</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Hard_to_relax</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>由于不安而无法静坐</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Unable_to_sit_still_due_to_restlessness</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">变得容易烦恼或急躁 </t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Become_easily_irritable_or_irritable</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>感到似乎将有可怕的事情发生而害怕</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Fear_that_something_terrible_is_about_to_happen</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>MAIN</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>QUESTIONNAIRE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data, image on 2022-04-143
</commit_message>
<xml_diff>
--- a/data/insomnia_and_sleep_quality_node.xlsx
+++ b/data/insomnia_and_sleep_quality_node.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3435" yWindow="4350" windowWidth="21600" windowHeight="11775" tabRatio="600" firstSheet="2" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5748" yWindow="1092" windowWidth="17280" windowHeight="9420" tabRatio="600" firstSheet="4" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MAIN" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INSOMNIA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MENOPAUSE_INSOMNIA" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GAD_7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ISI" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ANALYSIS" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -471,19 +473,19 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col width="20.875" customWidth="1" style="7" min="1" max="1"/>
-    <col width="18.875" customWidth="1" style="6" min="2" max="3"/>
-    <col width="14.875" customWidth="1" style="6" min="4" max="4"/>
+    <col width="20.8984375" customWidth="1" style="7" min="1" max="1"/>
+    <col width="18.8984375" customWidth="1" style="6" min="2" max="3"/>
+    <col width="14.8984375" customWidth="1" style="6" min="4" max="4"/>
     <col width="17" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
     <col width="32" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="11" customWidth="1" style="6" min="7" max="23"/>
-    <col width="11" customWidth="1" style="6" min="24" max="16384"/>
+    <col width="11" customWidth="1" style="6" min="7" max="31"/>
+    <col width="11" customWidth="1" style="6" min="32" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1648,16 +1650,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="23.25" customWidth="1" style="8" min="1" max="1"/>
-    <col width="21.25" customWidth="1" style="8" min="2" max="2"/>
+    <col width="23.19921875" customWidth="1" style="8" min="1" max="1"/>
+    <col width="21.19921875" customWidth="1" style="8" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="6">
@@ -3850,6 +3852,1332 @@
       <c r="C129" s="6" t="inlineStr">
         <is>
           <t>MAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B130" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C130" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B131" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C131" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B132" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C132" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B133" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C133" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B134" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C134" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B135" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C135" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B136" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C136" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B137" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C137" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B138" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C138" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B139" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C139" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B140" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C140" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B141" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C141" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B142" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C142" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B143" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C143" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B144" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C144" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B145" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C145" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B146" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C146" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B147" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C147" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B148" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C148" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B149" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C149" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B150" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C150" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B151" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C151" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B152" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C152" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B153" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C153" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="B154" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C154" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="B155" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C155" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="B156" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C156" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="B157" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C157" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_evaluation_no_mild_moderate_severe_</t>
+        </is>
+      </c>
+      <c r="B158" s="6" t="inlineStr">
+        <is>
+          <t>EVALUATION</t>
+        </is>
+      </c>
+      <c r="C158" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_EVALUATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="6" t="inlineStr">
+        <is>
+          <t>ISI_</t>
+        </is>
+      </c>
+      <c r="B159" s="6" t="inlineStr">
+        <is>
+          <t>QUESTIONNAIRE</t>
+        </is>
+      </c>
+      <c r="C159" s="6" t="inlineStr">
+        <is>
+          <t>MAIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="6" t="inlineStr">
+        <is>
+          <t>ISI_evaluation_mild_moderate_severe_</t>
+        </is>
+      </c>
+      <c r="B160" s="6" t="inlineStr">
+        <is>
+          <t>EVALUATION</t>
+        </is>
+      </c>
+      <c r="C160" s="6" t="inlineStr">
+        <is>
+          <t>ISI_EVALUATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="6" t="inlineStr">
+        <is>
+          <t>Difficulty_falling_asleep_in_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="B161" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C161" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="6" t="inlineStr">
+        <is>
+          <t>Difficulty_maintaining_sleep_over_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="B162" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C162" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="6" t="inlineStr">
+        <is>
+          <t>Woke_up_early_in_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="B163" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C163" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="6" t="inlineStr">
+        <is>
+          <t>Satisfaction_with_sleep_over_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="B164" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C164" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="6" t="inlineStr">
+        <is>
+          <t>How_much_sleep_problems_interfere_with_your_daily_activities</t>
+        </is>
+      </c>
+      <c r="B165" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C165" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="6" t="inlineStr">
+        <is>
+          <t>How_others_see_your_sleep_problems_affecting_your_quality_of_life</t>
+        </is>
+      </c>
+      <c r="B166" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C166" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="6" t="inlineStr">
+        <is>
+          <t>How_distressed_you_are_with_your_current_sleep_problems</t>
+        </is>
+      </c>
+      <c r="B167" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+      <c r="C167" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B168" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C168" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B169" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C169" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B170" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C170" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B171" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C171" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B172" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+      <c r="C172" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B173" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C173" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B174" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C174" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B175" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C175" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B176" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C176" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B177" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+      <c r="C177" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B178" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C178" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B179" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C179" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B180" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C180" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B181" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C181" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B182" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+      <c r="C182" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B183" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C183" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B184" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C184" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B185" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C185" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B186" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C186" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B187" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+      <c r="C187" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B188" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C188" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B189" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C189" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B190" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C190" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B191" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C191" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B192" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+      <c r="C192" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B193" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C193" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B194" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C194" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B195" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C195" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B196" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C196" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B197" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+      <c r="C197" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B198" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C198" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="B199" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C199" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="B200" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C200" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="B201" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C201" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="B202" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+      <c r="C202" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="6" t="inlineStr">
+        <is>
+          <t>Causes_of_insomnia</t>
+        </is>
+      </c>
+      <c r="B203" s="6" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+      <c r="C203" s="6" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="6" t="inlineStr">
+        <is>
+          <t>Lesion</t>
+        </is>
+      </c>
+      <c r="B204" s="6" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+      <c r="C204" s="6" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="6" t="inlineStr">
+        <is>
+          <t>Treatment_method</t>
+        </is>
+      </c>
+      <c r="B205" s="6" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+      <c r="C205" s="6" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="6" t="inlineStr">
+        <is>
+          <t>Possible_complications</t>
+        </is>
+      </c>
+      <c r="B206" s="6" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+      <c r="C206" s="6" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="6" t="inlineStr">
+        <is>
+          <t>Possible_symptoms</t>
+        </is>
+      </c>
+      <c r="B207" s="6" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+      <c r="C207" s="6" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
         </is>
       </c>
     </row>
@@ -3870,12 +5198,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="19.125" customWidth="1" style="8" min="1" max="1"/>
-    <col width="18.75" customWidth="1" style="8" min="2" max="2"/>
-    <col width="12.25" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.75" customWidth="1" style="8" min="4" max="4"/>
+    <col width="19.09765625" customWidth="1" style="8" min="1" max="1"/>
+    <col width="18.69921875" customWidth="1" style="8" min="2" max="2"/>
+    <col width="12.19921875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.69921875" customWidth="1" style="8" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4333,12 +5661,12 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
     <col width="19" customWidth="1" style="8" min="1" max="1"/>
     <col width="15.5" customWidth="1" style="8" min="2" max="2"/>
-    <col width="12.25" customWidth="1" style="8" min="3" max="3"/>
-    <col width="16.75" customWidth="1" style="8" min="5" max="5"/>
+    <col width="12.19921875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="16.69921875" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4620,16 +5948,16 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="20.625" customWidth="1" style="8" min="1" max="1"/>
-    <col width="15.75" customWidth="1" style="8" min="2" max="2"/>
-    <col width="8.75" customWidth="1" style="6" min="3" max="3"/>
-    <col width="22.625" customWidth="1" style="8" min="5" max="5"/>
+    <col width="20.59765625" customWidth="1" style="8" min="1" max="1"/>
+    <col width="15.69921875" customWidth="1" style="8" min="2" max="2"/>
+    <col width="8.69921875" customWidth="1" style="6" min="3" max="3"/>
+    <col width="22.59765625" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5302,11 +6630,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="23.25" customWidth="1" style="8" min="1" max="1"/>
-    <col width="25.75" customWidth="1" style="8" min="2" max="3"/>
-    <col width="34.75" customWidth="1" style="8" min="5" max="5"/>
+    <col width="23.19921875" customWidth="1" style="8" min="1" max="1"/>
+    <col width="25.69921875" customWidth="1" style="8" min="2" max="3"/>
+    <col width="34.69921875" customWidth="1" style="8" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5766,16 +7094,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="29.375" customWidth="1" style="8" min="1" max="1"/>
-    <col width="24.125" customWidth="1" style="8" min="2" max="2"/>
+    <col width="29.3984375" customWidth="1" style="8" min="1" max="1"/>
+    <col width="24.09765625" customWidth="1" style="8" min="2" max="2"/>
+    <col width="9.8984375" customWidth="1" style="8" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5986,8 +7315,1839 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E26" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E27" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E28" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E30" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E32" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">完全不会 </t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>Not_at_all</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E34" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>好几天</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>A_few_days</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E35" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>超过一周</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t>More_than_a_week</t>
+        </is>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E36" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>几乎每天</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>Almost_everyday</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_ANS</t>
+        </is>
+      </c>
+      <c r="E37" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7评估（没有_轻度_中度_重度）</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_evaluation_no_mild_moderate_severe_</t>
+        </is>
+      </c>
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>GAD_7_EVALUATION</t>
+        </is>
+      </c>
+      <c r="E38" s="6" t="inlineStr">
+        <is>
+          <t>EVALUATION</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="18.796875" customWidth="1" style="8" min="1" max="1"/>
+    <col width="17.3984375" customWidth="1" style="8" min="2" max="2"/>
+    <col width="11.5" customWidth="1" style="8" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>ChineseName</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>EnglishName</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Classification</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Abbreviation</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>CorrespondingReason</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>ISI_</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>ISI_</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>MAIN</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="n"/>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>QUESTIONNAIRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>ISI评估（没有_轻度_中度_重度）</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>ISI_evaluation_mild_moderate_severe_</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>ISI_EVALUATION</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>EVALUATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>在过去两个星期入睡困难</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Difficulty_falling_asleep_in_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>在过去两个星期难以维持睡眠</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Difficulty_maintaining_sleep_over_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>在过去两个星期很早就醒</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Woke_up_early_in_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>对过去两个星期的睡眠的满意度</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Satisfaction_with_sleep_over_the_past_two_weeks</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>睡眠问题对于您日常活动的妨碍程度</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>How_much_sleep_problems_interfere_with_your_daily_activities</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>在其他人眼中您的睡眠问题对您生活质量的影响程度</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>How_others_see_your_sleep_problems_affecting_your_quality_of_life</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>您对现在的睡眠问题的苦难程度</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>How_distressed_you_are_with_your_current_sleep_problems</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>QUESTION</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>ISI</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E19" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E25" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E26" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E27" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E28" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E30" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E32" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E34" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E35" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E36" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E37" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E38" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E39" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B40" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C40" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E40" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E41" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>轻微</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="inlineStr">
+        <is>
+          <t>Slight</t>
+        </is>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E42" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>普通</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>Ordinary</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E43" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="inlineStr">
+        <is>
+          <t>严重</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="inlineStr">
+        <is>
+          <t>Serious</t>
+        </is>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E44" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>非常严重</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>Very_serious</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>ISI_ANS</t>
+        </is>
+      </c>
+      <c r="E45" s="6" t="inlineStr">
+        <is>
+          <t>ISI_QUESTION_7</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
+  <cols>
+    <col width="16.796875" customWidth="1" style="8" min="1" max="1"/>
+    <col width="17.8984375" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.8984375" customWidth="1" style="8" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>ChineseName</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>EnglishName</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Classification</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Abbreviation</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>CorrespondingReason</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="6">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>失眠的原因</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Causes_of_insomnia</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="n"/>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>病灶</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Lesion</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>治疗方法</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Treatment_method</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>可能的并发症</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Possible_complications</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>可能的症状</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Possible_symptoms</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>FINAL_ANALYSIS</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>